<commit_message>
fuel boiler implemented in opt (ugly)
</commit_message>
<xml_diff>
--- a/data/input/Scenario_Component_Boiler.xlsx
+++ b/data/input/Scenario_Component_Boiler.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18400"/>
+    <workbookView windowWidth="30240" windowHeight="14720"/>
   </bookViews>
   <sheets>
     <sheet name="OperationScenario_Boiler" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12">
   <si>
     <t>ID_Boiler</t>
   </si>
@@ -48,18 +48,21 @@
   <si>
     <t>W</t>
   </si>
+  <si>
+    <t>gases</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -70,7 +73,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -83,13 +85,21 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -103,6 +113,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -110,9 +136,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -120,30 +160,44 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -157,39 +211,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -202,22 +225,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,192 +235,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor theme="8" tint="0.799981688894314"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -421,16 +436,38 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="8" tint="0.399975585192419"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color theme="8" tint="0.399975585192419"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8" tint="0.399975585192419"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="8" tint="0.399975585192419"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8" tint="0.399975585192419"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="8" tint="0.399975585192419"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="8" tint="0.399975585192419"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="8" tint="0.399975585192419"/>
       </bottom>
       <diagonal/>
     </border>
@@ -450,6 +487,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -465,11 +511,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -492,19 +555,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -512,161 +564,164 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -729,8 +784,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I2" totalsRowShown="0">
-  <autoFilter ref="A1:I2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I3" totalsRowShown="0">
+  <autoFilter ref="A1:I3"/>
   <tableColumns count="9">
     <tableColumn id="1" name="ID_Boiler"/>
     <tableColumn id="2" name="type"/>
@@ -1004,13 +1059,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="11.2890625" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -1080,6 +1135,35 @@
         <v>55</v>
       </c>
     </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
+        <v>15000</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2">
+        <v>7500</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="H3" s="2">
+        <v>35</v>
+      </c>
+      <c r="I3" s="3">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>